<commit_message>
refactor: streamline code formatting and improve readability across multiple files
</commit_message>
<xml_diff>
--- a/data/input/data_ground_truth_01/composicao.xlsx
+++ b/data/input/data_ground_truth_01/composicao.xlsx
@@ -242,14 +242,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1018" style="2" width="9.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="2" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>